<commit_message>
commit curtailments new analysis 2
</commit_message>
<xml_diff>
--- a/Wind Curtailment/New Analysis 01-06/apwindcurtailment.xlsx
+++ b/Wind Curtailment/New Analysis 01-06/apwindcurtailment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\POSOCO\AP Curtailment Analysis\Curtialment\Wind Curtailment\New Analysis 01-06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA338963-BC60-4708-915E-5F7C460C738E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A607D18C-44CD-4201-94D4-6215B594C215}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -715,11 +715,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E64F16BF-6AB7-4BD4-8985-31E7B2E9D8F2}">
   <dimension ref="A1:G410"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:I409"/>
+    <sheetView tabSelected="1" topLeftCell="A406" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">

</xml_diff>